<commit_message>
new seascape estimation code
</commit_message>
<xml_diff>
--- a/results/seascape_library.xlsx
+++ b/results/seascape_library.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -522,52 +522,52 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-2.227982843649738</v>
+        <v>-2.227982845564258</v>
       </c>
       <c r="C2" t="n">
-        <v>1.691542679178141</v>
+        <v>1.691542679133625</v>
       </c>
       <c r="D2" t="n">
-        <v>-0.01397775041401107</v>
+        <v>-0.01397772348117606</v>
       </c>
       <c r="E2" t="n">
-        <v>2.072901988491544</v>
+        <v>2.07290177865642</v>
       </c>
       <c r="F2" t="n">
-        <v>0.2890858619240341</v>
+        <v>0.289085714247282</v>
       </c>
       <c r="G2" t="n">
-        <v>2.559642142944998</v>
+        <v>2.559641999140384</v>
       </c>
       <c r="H2" t="n">
-        <v>-0.03485988711367522</v>
+        <v>-0.03485986136713184</v>
       </c>
       <c r="I2" t="n">
-        <v>2.742253360455529</v>
+        <v>2.74225335666608</v>
       </c>
       <c r="J2" t="n">
-        <v>-0.128338944143656</v>
+        <v>-0.1283315493251282</v>
       </c>
       <c r="K2" t="n">
-        <v>2.383750110079761</v>
+        <v>2.383750108297807</v>
       </c>
       <c r="L2" t="n">
-        <v>-0.8372295300887417</v>
+        <v>-0.8372326127871542</v>
       </c>
       <c r="M2" t="n">
-        <v>2.091717536304257</v>
+        <v>2.091717344108099</v>
       </c>
       <c r="N2" t="n">
-        <v>0.9900279771447263</v>
+        <v>0.9900279470093564</v>
       </c>
       <c r="O2" t="n">
-        <v>0.6065804681315971</v>
+        <v>0.6065804637285234</v>
       </c>
       <c r="P2" t="n">
-        <v>0.6179633139093655</v>
+        <v>0.6179633324363734</v>
       </c>
       <c r="Q2" t="n">
-        <v>2.695583879242885</v>
+        <v>2.695584445514665</v>
       </c>
     </row>
     <row r="3">
@@ -577,52 +577,52 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.08727773593513799</v>
+        <v>0.08727773682716269</v>
       </c>
       <c r="C3" t="n">
-        <v>0.07985922829535715</v>
+        <v>0.07985922828730303</v>
       </c>
       <c r="D3" t="n">
-        <v>0.09028212897165196</v>
+        <v>0.09028212941226556</v>
       </c>
       <c r="E3" t="n">
-        <v>0.1132130689170288</v>
+        <v>0.113213069835272</v>
       </c>
       <c r="F3" t="n">
-        <v>0.1003312022134434</v>
+        <v>0.1003312022132046</v>
       </c>
       <c r="G3" t="n">
-        <v>0.06886068677462256</v>
+        <v>0.06886068683503578</v>
       </c>
       <c r="H3" t="n">
-        <v>0.07671369895030068</v>
+        <v>0.07671369804858134</v>
       </c>
       <c r="I3" t="n">
-        <v>0.07747740233396851</v>
+        <v>0.07747740231909898</v>
       </c>
       <c r="J3" t="n">
-        <v>0.09747906883120511</v>
+        <v>0.09747906883412173</v>
       </c>
       <c r="K3" t="n">
-        <v>0.08252831858217921</v>
+        <v>0.08252831828963693</v>
       </c>
       <c r="L3" t="n">
-        <v>0.08079091136876933</v>
+        <v>0.08079091271599423</v>
       </c>
       <c r="M3" t="n">
-        <v>0.08121588399875594</v>
+        <v>0.08121588398253661</v>
       </c>
       <c r="N3" t="n">
-        <v>0.08752331889046973</v>
+        <v>0.08752331889278714</v>
       </c>
       <c r="O3" t="n">
-        <v>0.07218521343374412</v>
+        <v>0.072185213219539</v>
       </c>
       <c r="P3" t="n">
-        <v>0.06468702969491059</v>
+        <v>0.06468702969420353</v>
       </c>
       <c r="Q3" t="n">
-        <v>0.06815518332290832</v>
+        <v>0.06815518334342985</v>
       </c>
     </row>
     <row r="4">
@@ -632,52 +632,52 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-0.07293256834056713</v>
+        <v>-0.0729325690347343</v>
       </c>
       <c r="C4" t="n">
-        <v>-0.00152384874334747</v>
+        <v>-0.001523848729763579</v>
       </c>
       <c r="D4" t="n">
-        <v>-0.05124581786133297</v>
+        <v>-0.05124582542600568</v>
       </c>
       <c r="E4" t="n">
-        <v>-0.06602734628170322</v>
+        <v>-0.06602726764236053</v>
       </c>
       <c r="F4" t="n">
-        <v>-0.003910533467115913</v>
+        <v>-0.003910534994063236</v>
       </c>
       <c r="G4" t="n">
-        <v>-0.03671102292695302</v>
+        <v>-0.03671114734984983</v>
       </c>
       <c r="H4" t="n">
-        <v>-0.09938407944833326</v>
+        <v>-0.09938409118519045</v>
       </c>
       <c r="I4" t="n">
-        <v>-0.09612832852433062</v>
+        <v>-0.09612832635613419</v>
       </c>
       <c r="J4" t="n">
-        <v>-0.04062354694569258</v>
+        <v>-0.04062813463405443</v>
       </c>
       <c r="K4" t="n">
-        <v>-0.00270224618741589</v>
+        <v>-0.002702246598032611</v>
       </c>
       <c r="L4" t="n">
-        <v>-0.03885006684482412</v>
+        <v>-0.03884987071371173</v>
       </c>
       <c r="M4" t="n">
-        <v>-0.07364557480504348</v>
+        <v>-0.07364549959054111</v>
       </c>
       <c r="N4" t="n">
-        <v>-0.006937495598289802</v>
+        <v>-0.006937460060272815</v>
       </c>
       <c r="O4" t="n">
-        <v>-0.00195732650470061</v>
+        <v>-0.001957325023747557</v>
       </c>
       <c r="P4" t="n">
-        <v>-0.001408835895358641</v>
+        <v>-0.001408835895365335</v>
       </c>
       <c r="Q4" t="n">
-        <v>-0.04845972076953083</v>
+        <v>-0.04846001417319322</v>
       </c>
     </row>
   </sheetData>

</xml_diff>